<commit_message>
Reading data from file
</commit_message>
<xml_diff>
--- a/gamedata.xlsx
+++ b/gamedata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="0" windowWidth="25600" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="25600" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,38 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Total Points</t>
+  </si>
+  <si>
+    <t>Games Played</t>
+  </si>
+  <si>
+    <t>Wins</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
+    <t>Players</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Jasper</t>
+  </si>
+  <si>
+    <t>Nolan</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,13 +414,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>190</v>
+      </c>
+      <c r="E2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Save button is broken in a different way now
</commit_message>
<xml_diff>
--- a/gamedata.xlsx
+++ b/gamedata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Total Points</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>0/0/0/0/</t>
+  </si>
+  <si>
+    <t>1/1/</t>
+  </si>
+  <si>
+    <t>2/</t>
+  </si>
+  <si>
+    <t>3/3/3/3/3/</t>
   </si>
 </sst>
 </file>
@@ -472,68 +484,68 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>150</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>190</v>
-      </c>
-      <c r="E2">
-        <v>135</v>
+      <c r="B2" t="n">
+        <v>163.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>135.0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
+      <c r="B3" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="B4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>9</v>
+      <c r="B5" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>9.0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -541,16 +553,16 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
It isn’t broken at all now
</commit_message>
<xml_diff>
--- a/gamedata.xlsx
+++ b/gamedata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Total Points</t>
   </si>
@@ -51,28 +51,25 @@
     <t>Rolls</t>
   </si>
   <si>
-    <t>6/7/8</t>
-  </si>
-  <si>
-    <t>5/1</t>
-  </si>
-  <si>
-    <t>1/8/9/7/5</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>0/0/0/0/</t>
-  </si>
-  <si>
-    <t>1/1/</t>
+    <t>3/3/3/3/3/</t>
+  </si>
+  <si>
+    <t>5/12/5</t>
+  </si>
+  <si>
+    <t>7/25/3</t>
+  </si>
+  <si>
+    <t>5/12/5/16/</t>
   </si>
   <si>
     <t>2/</t>
   </si>
   <si>
-    <t>3/3/3/3/3/</t>
+    <t>7/25/3/</t>
   </si>
 </sst>
 </file>
@@ -458,7 +455,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -485,7 +482,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>163.0</v>
+        <v>179.0</v>
       </c>
       <c r="C2" t="n">
         <v>100.0</v>
@@ -562,16 +559,12 @@
         <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <ignoredErrors>
-    <ignoredError sqref="B6" twoDigitTextYear="1"/>
-    <ignoredError sqref="D6" numberStoredAsText="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>